<commit_message>
Fixed error and updated Test Plan
</commit_message>
<xml_diff>
--- a/test/atdd scenarios/Seminar Registration - ATDD Scenarios - SOLID.xlsx
+++ b/test/atdd scenarios/Seminar Registration - ATDD Scenarios - SOLID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Presentations/DOK/2024/Nordic/Presentation 1 - Tips ^0 Tricks for efficient and effective test automation data setup/Code Examples/Seminar Management/test/atdd scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="414" documentId="13_ncr:1_{1643C2B1-EA4C-4D1D-97AA-B1BFC59B4C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A96FC603-7D9B-4E1D-A2B2-9ECD618D6A06}"/>
+  <xr:revisionPtr revIDLastSave="491" documentId="13_ncr:1_{1643C2B1-EA4C-4D1D-97AA-B1BFC59B4C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72660801-F0A6-4914-89A4-A64F6794A9F5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27720" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27720" windowHeight="16440" activeTab="4" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="96">
   <si>
     <t>Feature</t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t>Check registration lines exist invalid</t>
+  </si>
+  <si>
+    <t>Registration</t>
   </si>
 </sst>
 </file>
@@ -349,7 +352,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -474,7 +476,19 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -482,18 +496,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -506,6 +508,13 @@
   </cellStyles>
   <dxfs count="60">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -543,13 +552,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1250,21 +1252,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C0055D-05C7-497B-B9D2-9B28D7DAD451}">
   <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:H95"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="62.85546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="38.42578125" style="6" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1409,7 +1413,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1480,7 +1484,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="6" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1500,7 +1504,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1534,7 +1538,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1551,7 +1555,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1688,7 +1692,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1728,7 +1732,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -1908,7 +1912,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2048,7 +2052,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -2088,7 +2092,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -2228,7 +2232,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -2268,7 +2272,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -2448,7 +2452,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -2468,7 +2472,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="28.5" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>11</v>
       </c>
@@ -2588,7 +2592,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -2628,7 +2632,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -2648,7 +2652,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="33" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>11</v>
       </c>
@@ -2768,7 +2772,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -2808,7 +2812,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>11</v>
       </c>
@@ -2908,7 +2912,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -3048,7 +3052,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>11</v>
       </c>
@@ -3320,24 +3324,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2411316F-A8C6-4656-8F70-D35B88200C70}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="49.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.85546875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="33.140625" style="6" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3506,7 +3510,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3589,7 +3593,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="6" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3612,7 +3616,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3632,7 +3636,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -3652,7 +3656,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -3672,7 +3676,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -3693,25 +3697,25 @@
       </c>
     </row>
     <row r="18" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="17" t="s">
+      <c r="A18" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="20" t="s">
         <v>89</v>
       </c>
       <c r="D18" s="21"/>
-      <c r="E18" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="17" t="s">
+      <c r="E18" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="20">
+      <c r="G18" s="20"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="24">
         <v>401</v>
       </c>
     </row>
@@ -3725,7 +3729,7 @@
       <c r="C19" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="22"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="10" t="s">
         <v>10</v>
       </c>
@@ -3748,7 +3752,7 @@
       <c r="C20" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="22"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="5" t="s">
         <v>10</v>
       </c>
@@ -3772,7 +3776,7 @@
       <c r="C21" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="22"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="5" t="s">
         <v>10</v>
       </c>
@@ -3796,7 +3800,7 @@
       <c r="C22" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="17"/>
       <c r="E22" s="5" t="s">
         <v>10</v>
       </c>
@@ -3820,7 +3824,7 @@
       <c r="C23" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="22"/>
+      <c r="D23" s="17"/>
       <c r="E23" s="5" t="s">
         <v>10</v>
       </c>
@@ -3844,7 +3848,7 @@
       <c r="C24" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="22"/>
+      <c r="D24" s="17"/>
       <c r="E24" s="5" t="s">
         <v>10</v>
       </c>
@@ -3858,7 +3862,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -3868,7 +3872,7 @@
       <c r="C25" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="22"/>
+      <c r="D25" s="17"/>
       <c r="E25" s="5" t="s">
         <v>10</v>
       </c>
@@ -3892,7 +3896,7 @@
       <c r="C26" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="22"/>
+      <c r="D26" s="17"/>
       <c r="E26" s="5" t="s">
         <v>10</v>
       </c>
@@ -3906,7 +3910,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -3916,7 +3920,7 @@
       <c r="C27" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="22"/>
+      <c r="D27" s="17"/>
       <c r="E27" s="5" t="s">
         <v>10</v>
       </c>
@@ -3931,117 +3935,117 @@
       </c>
     </row>
     <row r="28" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="17" t="s">
+      <c r="A28" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="20" t="s">
         <v>89</v>
       </c>
       <c r="D28" s="21"/>
-      <c r="E28" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="17" t="s">
+      <c r="E28" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="20">
+      <c r="G28" s="20"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="24">
         <v>403</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="17" t="s">
+      <c r="A29" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="20" t="s">
         <v>89</v>
       </c>
       <c r="D29" s="21"/>
-      <c r="E29" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="17" t="s">
+      <c r="E29" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="20">
+      <c r="G29" s="20"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="24">
         <v>404</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="17" t="s">
+      <c r="A30" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="20" t="s">
         <v>89</v>
       </c>
       <c r="D30" s="21"/>
-      <c r="E30" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="17" t="s">
+      <c r="E30" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="20">
+      <c r="G30" s="20"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="24">
         <v>405</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="17" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="20" t="s">
         <v>89</v>
       </c>
       <c r="D31" s="21"/>
-      <c r="E31" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="17" t="s">
+      <c r="E31" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="G31" s="17"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="20">
+      <c r="G31" s="20"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="24">
         <v>406</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="17" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="20" t="s">
         <v>89</v>
       </c>
       <c r="D32" s="21"/>
-      <c r="E32" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="17" t="s">
+      <c r="E32" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G32" s="17"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="20">
+      <c r="G32" s="20"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="24">
         <v>407</v>
       </c>
     </row>
@@ -4055,7 +4059,7 @@
       <c r="C33" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="23"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="10" t="s">
         <v>10</v>
       </c>
@@ -4078,7 +4082,7 @@
       <c r="C34" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="23"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="5" t="s">
         <v>10</v>
       </c>
@@ -4102,7 +4106,7 @@
       <c r="C35" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="23"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="5" t="s">
         <v>10</v>
       </c>
@@ -4126,7 +4130,7 @@
       <c r="C36" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="23"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="5" t="s">
         <v>10</v>
       </c>
@@ -4140,7 +4144,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -4150,7 +4154,7 @@
       <c r="C37" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="23"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="5" t="s">
         <v>10</v>
       </c>
@@ -4174,7 +4178,7 @@
       <c r="C38" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="23"/>
+      <c r="D38" s="18"/>
       <c r="E38" s="5" t="s">
         <v>10</v>
       </c>
@@ -4198,7 +4202,7 @@
       <c r="C39" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="23"/>
+      <c r="D39" s="18"/>
       <c r="E39" s="5" t="s">
         <v>10</v>
       </c>
@@ -4222,7 +4226,7 @@
       <c r="C40" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D40" s="24"/>
+      <c r="D40" s="19"/>
       <c r="E40" s="10" t="s">
         <v>10</v>
       </c>
@@ -4245,7 +4249,7 @@
       <c r="C41" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="24"/>
+      <c r="D41" s="19"/>
       <c r="E41" s="5" t="s">
         <v>10</v>
       </c>
@@ -4269,7 +4273,7 @@
       <c r="C42" t="s">
         <v>88</v>
       </c>
-      <c r="D42" s="24"/>
+      <c r="D42" s="19"/>
       <c r="E42" s="5" t="s">
         <v>10</v>
       </c>
@@ -4293,7 +4297,7 @@
       <c r="C43" t="s">
         <v>88</v>
       </c>
-      <c r="D43" s="24"/>
+      <c r="D43" s="19"/>
       <c r="E43" s="5" t="s">
         <v>10</v>
       </c>
@@ -4307,7 +4311,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -4317,7 +4321,7 @@
       <c r="C44" t="s">
         <v>88</v>
       </c>
-      <c r="D44" s="24"/>
+      <c r="D44" s="19"/>
       <c r="E44" s="5" t="s">
         <v>10</v>
       </c>
@@ -4341,7 +4345,7 @@
       <c r="C45" t="s">
         <v>88</v>
       </c>
-      <c r="D45" s="24"/>
+      <c r="D45" s="19"/>
       <c r="E45" s="5" t="s">
         <v>10</v>
       </c>
@@ -4365,7 +4369,7 @@
       <c r="C46" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="24"/>
+      <c r="D46" s="19"/>
       <c r="E46" s="5" t="s">
         <v>10</v>
       </c>
@@ -4380,25 +4384,25 @@
       </c>
     </row>
     <row r="47" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" s="17" t="s">
+      <c r="A47" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="20" t="s">
         <v>89</v>
       </c>
       <c r="D47" s="25"/>
-      <c r="E47" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" s="17" t="s">
+      <c r="E47" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="G47" s="17"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="20">
+      <c r="G47" s="20"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="24">
         <v>410</v>
       </c>
     </row>
@@ -4453,21 +4457,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075BFE33-317D-404C-B75F-6D8E2F4A55EC}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:H30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="61.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="36.5703125" style="6" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4495,12 +4501,12 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
@@ -4513,12 +4519,12 @@
     </row>
     <row r="3" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
@@ -4531,12 +4537,12 @@
     </row>
     <row r="4" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
@@ -4549,12 +4555,12 @@
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
@@ -4567,12 +4573,12 @@
     </row>
     <row r="6" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="10" t="s">
         <v>10</v>
       </c>
@@ -4585,12 +4591,12 @@
     </row>
     <row r="7" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
@@ -4603,12 +4609,12 @@
     </row>
     <row r="8" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
@@ -4621,12 +4627,12 @@
     </row>
     <row r="9" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
@@ -4639,12 +4645,12 @@
     </row>
     <row r="10" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="10" t="s">
         <v>10</v>
       </c>
@@ -4657,12 +4663,12 @@
     </row>
     <row r="11" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
@@ -4675,12 +4681,12 @@
     </row>
     <row r="12" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="5" t="s">
         <v>10</v>
       </c>
@@ -4693,12 +4699,12 @@
     </row>
     <row r="13" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
@@ -4711,12 +4717,12 @@
     </row>
     <row r="14" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="10" t="s">
         <v>10</v>
       </c>
@@ -4729,12 +4735,12 @@
     </row>
     <row r="15" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="22"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="5" t="s">
         <v>10</v>
       </c>
@@ -4747,12 +4753,12 @@
     </row>
     <row r="16" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B16" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="22"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="5" t="s">
         <v>10</v>
       </c>
@@ -4765,12 +4771,12 @@
     </row>
     <row r="17" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B17" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="5" t="s">
         <v>10</v>
       </c>
@@ -4783,12 +4789,12 @@
     </row>
     <row r="18" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="10" t="s">
         <v>10</v>
       </c>
@@ -4801,12 +4807,12 @@
     </row>
     <row r="19" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="22"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="5" t="s">
         <v>10</v>
       </c>
@@ -4819,12 +4825,12 @@
     </row>
     <row r="20" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B20" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="22"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="5" t="s">
         <v>10</v>
       </c>
@@ -4837,12 +4843,12 @@
     </row>
     <row r="21" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B21" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="22"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="5" t="s">
         <v>10</v>
       </c>
@@ -4855,12 +4861,12 @@
     </row>
     <row r="22" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="22"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="10" t="s">
         <v>10</v>
       </c>
@@ -4873,12 +4879,12 @@
     </row>
     <row r="23" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="22"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="5" t="s">
         <v>10</v>
       </c>
@@ -4891,12 +4897,12 @@
     </row>
     <row r="24" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B24" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="22"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="5" t="s">
         <v>10</v>
       </c>
@@ -4909,12 +4915,12 @@
     </row>
     <row r="25" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B25" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="22"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="5" t="s">
         <v>10</v>
       </c>
@@ -4927,12 +4933,12 @@
     </row>
     <row r="26" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="22"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="10" t="s">
         <v>10</v>
       </c>
@@ -4945,12 +4951,12 @@
     </row>
     <row r="27" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="22"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="5" t="s">
         <v>10</v>
       </c>
@@ -4963,12 +4969,12 @@
     </row>
     <row r="28" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="22"/>
+      <c r="C28" s="17"/>
       <c r="D28" s="5" t="s">
         <v>10</v>
       </c>
@@ -4981,12 +4987,12 @@
     </row>
     <row r="29" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B29" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="22"/>
+      <c r="C29" s="17"/>
       <c r="D29" s="5" t="s">
         <v>10</v>
       </c>
@@ -4999,12 +5005,12 @@
     </row>
     <row r="30" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="22"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="10"/>
       <c r="E30" s="9" t="s">
         <v>63</v>
@@ -5015,12 +5021,12 @@
     </row>
     <row r="31" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="22"/>
+      <c r="C31" s="17"/>
       <c r="F31" t="s">
         <v>7</v>
       </c>
@@ -5030,12 +5036,12 @@
     </row>
     <row r="32" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B32" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="22"/>
+      <c r="C32" s="17"/>
       <c r="F32" t="s">
         <v>8</v>
       </c>
@@ -5045,12 +5051,12 @@
     </row>
     <row r="33" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B33" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="22"/>
+      <c r="C33" s="17"/>
       <c r="F33" t="s">
         <v>9</v>
       </c>
@@ -5110,21 +5116,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724597F8-7F07-4837-8513-9B9A72529247}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="67.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="36.5703125" style="6" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5152,12 +5160,12 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="23"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
@@ -5170,12 +5178,12 @@
     </row>
     <row r="3" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
@@ -5188,12 +5196,12 @@
     </row>
     <row r="4" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="23"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
@@ -5206,12 +5214,12 @@
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="23"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
@@ -5224,12 +5232,12 @@
     </row>
     <row r="6" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="23"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="10" t="s">
         <v>10</v>
       </c>
@@ -5242,12 +5250,12 @@
     </row>
     <row r="7" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="23"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
@@ -5260,12 +5268,12 @@
     </row>
     <row r="8" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="23"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
@@ -5278,12 +5286,12 @@
     </row>
     <row r="9" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="23"/>
+      <c r="C9" s="18"/>
       <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
@@ -5296,12 +5304,12 @@
     </row>
     <row r="10" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="23"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="10"/>
       <c r="E10" s="9" t="s">
         <v>68</v>
@@ -5312,12 +5320,12 @@
     </row>
     <row r="11" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="18"/>
       <c r="F11" t="s">
         <v>7</v>
       </c>
@@ -5327,12 +5335,12 @@
     </row>
     <row r="12" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="23"/>
+      <c r="C12" s="18"/>
       <c r="F12" t="s">
         <v>8</v>
       </c>
@@ -5342,12 +5350,12 @@
     </row>
     <row r="13" spans="1:8" s="7" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="5"/>
       <c r="E13"/>
       <c r="F13" t="s">
@@ -5409,21 +5417,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B9C6DB-C620-466B-AEDE-423C3007F697}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="62.85546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="36.5703125" style="6" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5451,12 +5461,12 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="23"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
@@ -5469,12 +5479,12 @@
     </row>
     <row r="3" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
@@ -5487,12 +5497,12 @@
     </row>
     <row r="4" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="23"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
@@ -5505,12 +5515,12 @@
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="23"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
@@ -5523,12 +5533,12 @@
     </row>
     <row r="6" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="24"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="10"/>
       <c r="E6" s="9" t="s">
         <v>94</v>
@@ -5539,12 +5549,12 @@
     </row>
     <row r="7" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="24"/>
+      <c r="C7" s="19"/>
       <c r="F7" t="s">
         <v>7</v>
       </c>
@@ -5554,12 +5564,12 @@
     </row>
     <row r="8" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="24"/>
+      <c r="C8" s="19"/>
       <c r="F8" t="s">
         <v>8</v>
       </c>
@@ -5569,12 +5579,12 @@
     </row>
     <row r="9" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="24"/>
+      <c r="C9" s="19"/>
       <c r="F9" t="s">
         <v>9</v>
       </c>
@@ -5585,28 +5595,28 @@
     <row r="10" spans="1:8" collapsed="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsBlanks" dxfId="5" priority="5">
+    <cfRule type="containsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Changes to Test Plan, fixed some compiler directives
</commit_message>
<xml_diff>
--- a/test/atdd scenarios/Seminar Registration - ATDD Scenarios - SOLID.xlsx
+++ b/test/atdd scenarios/Seminar Registration - ATDD Scenarios - SOLID.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Presentations/DOK/2024/Nordic/Presentation 1 - Tips ^0 Tricks for efficient and effective test automation data setup/Code Examples/Seminar Management/test/atdd scenarios/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Presentations/Areopa Webinars/20240916 - On lightning-fast test automation^J SOLIDized code and a revised test plan/Code Examples/Seminar Management/test/atdd scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="491" documentId="13_ncr:1_{1643C2B1-EA4C-4D1D-97AA-B1BFC59B4C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72660801-F0A6-4914-89A4-A64F6794A9F5}"/>
+  <xr:revisionPtr revIDLastSave="535" documentId="13_ncr:1_{1643C2B1-EA4C-4D1D-97AA-B1BFC59B4C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4353631C-26C1-4E95-B800-68AE6E924442}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27720" windowHeight="16440" activeTab="4" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="97">
   <si>
     <t>Feature</t>
   </si>
@@ -304,9 +304,6 @@
     <t>Usage</t>
   </si>
   <si>
-    <t>Implementation</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
@@ -326,6 +323,12 @@
   </si>
   <si>
     <t>Registration</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Flow</t>
   </si>
 </sst>
 </file>
@@ -335,7 +338,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +357,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -430,7 +440,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -501,19 +511,22 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="60">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -552,6 +565,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -885,8 +905,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6194755E-8EAD-4A4B-B309-823EE8CF2A94}" name="Table2932" displayName="Table2932" ref="A1:I47" totalsRowShown="0" headerRowDxfId="53">
-  <autoFilter ref="A1:I47" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6194755E-8EAD-4A4B-B309-823EE8CF2A94}" name="Table2932" displayName="Table2932" ref="A1:I13" totalsRowShown="0" headerRowDxfId="53">
+  <autoFilter ref="A1:I13" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD35BB68-F025-482D-97BF-90C020CBA765}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{2229E81B-30C1-4630-B967-B326EFC4B902}" name="Sub Feature"/>
@@ -1253,7 +1273,7 @@
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:H95"/>
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -3322,13 +3342,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2411316F-A8C6-4656-8F70-D35B88200C70}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:I47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -3378,7 +3398,7 @@
         <v>65</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
@@ -3390,1019 +3410,253 @@
       <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="26"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="29">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" s="21"/>
+      <c r="E4" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="20"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" s="17"/>
+      <c r="E5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="24">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="20"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="24">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" s="21"/>
+      <c r="E7" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="20"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="24">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="G7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" s="21"/>
+      <c r="E8" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" s="21"/>
+      <c r="E9" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" s="21"/>
+      <c r="E10" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" s="18"/>
+      <c r="E11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="24">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" s="19"/>
+      <c r="E12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="24">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12"/>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13"/>
-      <c r="G13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" t="s">
-        <v>88</v>
-      </c>
-      <c r="G14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="24">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="12">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20" s="12">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="12">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="12">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23" s="12">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="12">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="12">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I26" s="12">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I27" s="12">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" s="20"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="24">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="21"/>
-      <c r="E29" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="G29" s="20"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="24">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G30" s="20"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="24">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="20"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="24">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="G32" s="20"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="24">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G33" s="9"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="12">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" t="s">
-        <v>88</v>
-      </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I34" s="7">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="7">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="18"/>
-      <c r="E36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I36" s="7">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I37" s="7">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" t="s">
-        <v>84</v>
-      </c>
-      <c r="C38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="7">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" t="s">
-        <v>88</v>
-      </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" t="s">
-        <v>9</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I39" s="7">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" s="19"/>
-      <c r="E40" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="12">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G41" t="s">
-        <v>7</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I41" s="7">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="19"/>
-      <c r="E42" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G42" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I42" s="7">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="19"/>
-      <c r="E43" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G43" t="s">
-        <v>7</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I43" s="7">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44" t="s">
-        <v>88</v>
-      </c>
-      <c r="D44" s="19"/>
-      <c r="E44" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G44" t="s">
-        <v>7</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I44" s="7">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G45" t="s">
-        <v>8</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I45" s="7">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" s="19"/>
-      <c r="E46" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G46" t="s">
-        <v>9</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I46" s="7">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" s="25"/>
-      <c r="E47" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" s="20" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="G47" s="20"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="24">
+      <c r="G13" s="20"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="24">
         <v>410</v>
       </c>
     </row>
@@ -4501,7 +3755,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>64</v>
@@ -4519,7 +3773,7 @@
     </row>
     <row r="3" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
         <v>64</v>
@@ -4537,7 +3791,7 @@
     </row>
     <row r="4" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>64</v>
@@ -4555,7 +3809,7 @@
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
         <v>64</v>
@@ -4573,7 +3827,7 @@
     </row>
     <row r="6" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>64</v>
@@ -4591,7 +3845,7 @@
     </row>
     <row r="7" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
         <v>64</v>
@@ -4609,7 +3863,7 @@
     </row>
     <row r="8" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
         <v>64</v>
@@ -4627,7 +3881,7 @@
     </row>
     <row r="9" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
         <v>64</v>
@@ -4645,7 +3899,7 @@
     </row>
     <row r="10" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>64</v>
@@ -4663,7 +3917,7 @@
     </row>
     <row r="11" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
@@ -4681,7 +3935,7 @@
     </row>
     <row r="12" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" t="s">
         <v>64</v>
@@ -4699,7 +3953,7 @@
     </row>
     <row r="13" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
         <v>64</v>
@@ -4717,7 +3971,7 @@
     </row>
     <row r="14" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>64</v>
@@ -4735,7 +3989,7 @@
     </row>
     <row r="15" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
         <v>64</v>
@@ -4753,7 +4007,7 @@
     </row>
     <row r="16" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
         <v>64</v>
@@ -4771,7 +4025,7 @@
     </row>
     <row r="17" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
         <v>64</v>
@@ -4789,7 +4043,7 @@
     </row>
     <row r="18" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>64</v>
@@ -4807,7 +4061,7 @@
     </row>
     <row r="19" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
         <v>64</v>
@@ -4825,7 +4079,7 @@
     </row>
     <row r="20" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
         <v>64</v>
@@ -4843,7 +4097,7 @@
     </row>
     <row r="21" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
         <v>64</v>
@@ -4861,7 +4115,7 @@
     </row>
     <row r="22" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>64</v>
@@ -4879,7 +4133,7 @@
     </row>
     <row r="23" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
         <v>64</v>
@@ -4897,7 +4151,7 @@
     </row>
     <row r="24" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
         <v>64</v>
@@ -4915,7 +4169,7 @@
     </row>
     <row r="25" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" t="s">
         <v>64</v>
@@ -4933,7 +4187,7 @@
     </row>
     <row r="26" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>64</v>
@@ -4951,7 +4205,7 @@
     </row>
     <row r="27" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
         <v>64</v>
@@ -4969,7 +4223,7 @@
     </row>
     <row r="28" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
         <v>64</v>
@@ -4987,7 +4241,7 @@
     </row>
     <row r="29" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B29" t="s">
         <v>64</v>
@@ -5005,7 +4259,7 @@
     </row>
     <row r="30" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>64</v>
@@ -5021,7 +4275,7 @@
     </row>
     <row r="31" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
         <v>64</v>
@@ -5036,7 +4290,7 @@
     </row>
     <row r="32" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" t="s">
         <v>64</v>
@@ -5051,7 +4305,7 @@
     </row>
     <row r="33" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B33" t="s">
         <v>64</v>
@@ -5160,7 +4414,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>84</v>
@@ -5178,7 +4432,7 @@
     </row>
     <row r="3" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
         <v>84</v>
@@ -5196,7 +4450,7 @@
     </row>
     <row r="4" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>84</v>
@@ -5214,7 +4468,7 @@
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
         <v>84</v>
@@ -5232,7 +4486,7 @@
     </row>
     <row r="6" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>84</v>
@@ -5250,7 +4504,7 @@
     </row>
     <row r="7" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
         <v>84</v>
@@ -5268,7 +4522,7 @@
     </row>
     <row r="8" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
         <v>84</v>
@@ -5286,7 +4540,7 @@
     </row>
     <row r="9" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
         <v>84</v>
@@ -5304,7 +4558,7 @@
     </row>
     <row r="10" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>84</v>
@@ -5320,7 +4574,7 @@
     </row>
     <row r="11" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
         <v>84</v>
@@ -5335,7 +4589,7 @@
     </row>
     <row r="12" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" t="s">
         <v>84</v>
@@ -5350,7 +4604,7 @@
     </row>
     <row r="13" spans="1:8" s="7" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
         <v>84</v>
@@ -5417,7 +4671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B9C6DB-C620-466B-AEDE-423C3007F697}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -5461,7 +4715,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>84</v>
@@ -5471,7 +4725,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="11"/>
@@ -5479,7 +4733,7 @@
     </row>
     <row r="3" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
         <v>84</v>
@@ -5492,12 +4746,12 @@
         <v>7</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>84</v>
@@ -5510,12 +4764,12 @@
         <v>8</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
         <v>84</v>
@@ -5533,7 +4787,7 @@
     </row>
     <row r="6" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>84</v>
@@ -5541,7 +4795,7 @@
       <c r="C6" s="19"/>
       <c r="D6" s="10"/>
       <c r="E6" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="11"/>
@@ -5549,7 +4803,7 @@
     </row>
     <row r="7" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
         <v>84</v>
@@ -5559,12 +4813,12 @@
         <v>7</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
         <v>84</v>
@@ -5574,12 +4828,12 @@
         <v>8</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
         <v>84</v>
@@ -5595,28 +4849,28 @@
     <row r="10" spans="1:8" collapsed="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsBlanks" dxfId="0" priority="5">
+    <cfRule type="containsBlanks" dxfId="5" priority="5">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>